<commit_message>
Water Model Excel templates
</commit_message>
<xml_diff>
--- a/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
+++ b/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Water-Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1ED29E9E-FA61-45D2-843D-56F3BF982C18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{89881922-8C65-44C5-B038-E8BB21F73733}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
     <sheet name="Keywords" sheetId="21" r:id="rId2"/>
     <sheet name="KeywordsList" sheetId="36" state="hidden" r:id="rId3"/>
-    <sheet name="BondPotential-Harmonic" sheetId="1" r:id="rId4"/>
+    <sheet name="WaterModel-3Site-Rigid" sheetId="1" r:id="rId4"/>
+    <sheet name="WaterModel-4Site-Rigid" sheetId="37" r:id="rId5"/>
+    <sheet name="WaterModel-5Site-Rigid" sheetId="38" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -39,34 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
-  <si>
-    <t>Harmonic</t>
-  </si>
-  <si>
-    <t>K*(R-R0)^2</t>
-  </si>
-  <si>
-    <t>K-units</t>
-  </si>
-  <si>
-    <t>R0-units</t>
-  </si>
-  <si>
-    <t>AT-1</t>
-  </si>
-  <si>
-    <t>AT-2</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>R0</t>
-  </si>
-  <si>
-    <t>Bond Potential</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
   <si>
     <t># Preset</t>
   </si>
@@ -116,9 +91,6 @@
     <t>Force-Field Metadata</t>
   </si>
   <si>
-    <t>style</t>
-  </si>
-  <si>
     <t>formula</t>
   </si>
   <si>
@@ -128,15 +100,6 @@
     <t>version</t>
   </si>
   <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>kJ/mol/nm^2</t>
-  </si>
-  <si>
-    <t>nm</t>
-  </si>
-  <si>
     <t>Acetals</t>
   </si>
   <si>
@@ -363,6 +326,105 @@
   </si>
   <si>
     <t>Data Contact (Name)</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ROH-units</t>
+  </si>
+  <si>
+    <t>Å</t>
+  </si>
+  <si>
+    <t>Theta_HOH-units</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>epsilon-units</t>
+  </si>
+  <si>
+    <t>kJ/mol</t>
+  </si>
+  <si>
+    <t>A-units</t>
+  </si>
+  <si>
+    <t>B-units</t>
+  </si>
+  <si>
+    <t>sigma-units</t>
+  </si>
+  <si>
+    <t>x10^-3 (kcal*Å^12)/mol</t>
+  </si>
+  <si>
+    <t>(kcal*Å^6)/mol</t>
+  </si>
+  <si>
+    <t># Input</t>
+  </si>
+  <si>
+    <t>R_OH</t>
+  </si>
+  <si>
+    <t>Theta_HOH</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>q_O</t>
+  </si>
+  <si>
+    <t>q_H</t>
+  </si>
+  <si>
+    <t>EnergyDispersion</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>epsilon</t>
+  </si>
+  <si>
+    <t>Water Model</t>
+  </si>
+  <si>
+    <t>E=E_q+E_LJ</t>
+  </si>
+  <si>
+    <t>R-units</t>
+  </si>
+  <si>
+    <t>R_OM</t>
+  </si>
+  <si>
+    <t>q_M</t>
+  </si>
+  <si>
+    <t>Theta-units</t>
+  </si>
+  <si>
+    <t>R_OL</t>
+  </si>
+  <si>
+    <t>Theta_LOL</t>
+  </si>
+  <si>
+    <t>q_L</t>
+  </si>
+  <si>
+    <t>R-L</t>
+  </si>
+  <si>
+    <t>R-ij</t>
   </si>
 </sst>
 </file>
@@ -593,7 +655,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -661,6 +723,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1026,7 +1089,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="33" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B1" s="33"/>
     </row>
@@ -1036,7 +1099,7 @@
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" s="28"/>
     </row>
@@ -1046,73 +1109,73 @@
     </row>
     <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B6" s="32"/>
     </row>
     <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B8" s="25"/>
     </row>
     <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B9" s="25"/>
     </row>
     <row r="10" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B10" s="26"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B11" s="27"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B12" s="27"/>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B13" s="25"/>
     </row>
     <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B14" s="27"/>
     </row>
     <row r="15" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B15" s="27"/>
     </row>
     <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B16" s="30"/>
     </row>
@@ -1154,7 +1217,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B1" s="34"/>
     </row>
@@ -1163,7 +1226,7 @@
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5"/>
     </row>
@@ -1173,10 +1236,10 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,372 +1377,372 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1690,30 +1753,30 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="29"/>
+    <col min="3" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="33" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -1721,124 +1784,874 @@
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>29</v>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>"Harmonic"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0300-000001000000}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"K*(R-R0)^2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0300-000002000000}">
-      <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{00000000-0002-0000-0300-000002000000}">
+      <formula1>"Å"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-0300-000003000000}">
-      <formula1>"?, Å, nm"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{00000000-0002-0000-0300-000003000000}">
+      <formula1>"degrees"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{C78CE089-9E6A-40C4-9141-C58C935A20BC}">
+      <formula1>"kJ/mol, kcal/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{C0D946F8-3D9F-4F24-B64D-2A91F40BD84D}">
+      <formula1>"x10^-3 (kcal*Å^12)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{EC027274-46E4-4052-8494-9C3B981827CE}">
+      <formula1>"(kcal*Å^6)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{8AE6FBBD-7CF6-4C23-89D0-FA7A415546B4}">
+      <formula1>"Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{9EFB192C-4139-47D6-8D29-C4B68C0E2BCA}">
+      <formula1>"E=E_q+E_LJ, E=E_q+E_LJ+E_pol"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA409BC-7E78-4597-8B05-CA0A4A659430}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{46F2FA2B-D266-48AB-84A6-EA2AFF3A614D}">
+      <formula1>"Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{B15A06EE-54AD-4082-93A1-3C0AA4724878}">
+      <formula1>"(kcal*Å^6)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{B6C797B8-31DE-49AA-AA93-90CDB9967711}">
+      <formula1>"x10^-3 (kcal*Å^12)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{CE54A3E7-23E5-451E-8364-3D2340418811}">
+      <formula1>"kJ/mol, kcal/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{6A0608CF-AE06-4ABB-88BC-0EF511007B65}">
+      <formula1>"degrees"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{9F612AD7-D87E-4C27-93DA-B1520A82EF1C}">
+      <formula1>"K*(R-R0)^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{F87230C7-BEE8-4CF5-B887-89C07EB48F2D}">
+      <formula1>"E=E_q+E_LJ"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9" xr:uid="{F83F3F53-2845-40FD-BCBA-63099042DFC7}">
+      <formula1>"Å"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6173248F-86A5-4F55-B24D-4513AEE2F317}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="6" width="18" customWidth="1"/>
+    <col min="7" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9" xr:uid="{CFC99D1A-0498-4B8F-BBAC-0BC90AC8FCA3}">
+      <formula1>"Å"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{41976209-EECE-4A15-902C-16B110317682}">
+      <formula1>"E=E_q+E_LJ, E=S(R_ij)*E_q+E_LJ"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{433915BC-897E-4BAD-B9FC-072599DE43F9}">
+      <formula1>"K*(R-R0)^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{6299AA35-F5A0-4AD2-85FA-1E13F51C2ACD}">
+      <formula1>"degrees"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{852E5969-AF95-4E14-A03C-ACC0F089379C}">
+      <formula1>"kJ/mol, kcal/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{71BE57D9-129F-4125-B7E7-FEC4336611D7}">
+      <formula1>"x10^-3 (kcal*Å^12)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{7CB7972E-AEEF-4F7C-A3D7-B75477EE0135}">
+      <formula1>"(kcal*Å^6)/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{E9D5F352-08A0-4CA7-A962-8B0BC78823C8}">
+      <formula1>"Å, nm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished Water Models (Excel, XML, Python, and RSTs)
</commit_message>
<xml_diff>
--- a/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
+++ b/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Water-Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{89881922-8C65-44C5-B038-E8BB21F73733}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D0FF9E8E-6529-4EB9-B64B-2C6DDAB45D72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -331,9 +331,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>ROH-units</t>
-  </si>
-  <si>
     <t>Å</t>
   </si>
   <si>
@@ -425,6 +422,9 @@
   </si>
   <si>
     <t>R-ij</t>
+  </si>
+  <si>
+    <t>R-OH-units</t>
   </si>
 </sst>
 </file>
@@ -717,13 +717,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1088,10 +1088,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1216,10 +1216,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1757,9 +1757,9 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,17 +1775,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="A1" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1818,7 +1818,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -1831,12 +1831,12 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1846,12 +1846,12 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1862,10 +1862,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -1879,10 +1879,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -1930,10 +1930,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -1947,10 +1947,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1975,31 +1975,31 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="H14" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="I14" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2062,17 +2062,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="A1" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2091,7 +2091,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2105,7 +2105,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
@@ -2118,12 +2118,12 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2133,12 +2133,12 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2149,10 +2149,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -2183,10 +2183,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -2200,10 +2200,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -2217,10 +2217,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -2234,10 +2234,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -2262,31 +2262,31 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>121</v>
-      </c>
       <c r="G14" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2331,7 +2331,7 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
@@ -2349,20 +2349,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="A1" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2401,7 +2401,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
@@ -2417,12 +2417,12 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2435,12 +2435,12 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2454,10 +2454,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -2474,10 +2474,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -2534,10 +2534,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -2588,40 +2588,40 @@
     </row>
     <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="F14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="15" t="s">
-        <v>127</v>
-      </c>
       <c r="K14" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="L14" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated water model template
</commit_message>
<xml_diff>
--- a/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
+++ b/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Water-Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D0FF9E8E-6529-4EB9-B64B-2C6DDAB45D72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72039C4-F4BD-47C8-9C53-26D672D1532F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="20" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="40" r:id="rId1"/>
     <sheet name="Keywords" sheetId="21" r:id="rId2"/>
     <sheet name="KeywordsList" sheetId="36" state="hidden" r:id="rId3"/>
-    <sheet name="WaterModel-3Site-Rigid" sheetId="1" r:id="rId4"/>
-    <sheet name="WaterModel-4Site-Rigid" sheetId="37" r:id="rId5"/>
-    <sheet name="WaterModel-5Site-Rigid" sheetId="38" r:id="rId6"/>
+    <sheet name="References" sheetId="39" r:id="rId4"/>
+    <sheet name="WaterModel-3Site-Rigid" sheetId="1" r:id="rId5"/>
+    <sheet name="WaterModel-4Site-Rigid" sheetId="37" r:id="rId6"/>
+    <sheet name="WaterModel-5Site-Rigid" sheetId="38" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="134">
   <si>
     <t># Preset</t>
   </si>
@@ -58,9 +59,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Protocol</t>
-  </si>
-  <si>
     <t>Keywords</t>
   </si>
   <si>
@@ -319,9 +317,6 @@
     <t>- Silicon compounds</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -425,6 +420,30 @@
   </si>
   <si>
     <t>R-OH-units</t>
+  </si>
+  <si>
+    <t>Additional References</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Schema Version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Force-Field Protocol</t>
   </si>
 </sst>
 </file>
@@ -530,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -646,6 +665,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -655,7 +711,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -692,9 +748,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -723,6 +776,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1070,28 +1153,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DE7C7C-61A5-4979-9879-290B3550C46F}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" style="21" customWidth="1"/>
-    <col min="2" max="2" width="52" style="21" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" style="21" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1099,9 +1182,9 @@
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="28"/>
+        <v>12</v>
+      </c>
+      <c r="B3" s="27"/>
     </row>
     <row r="4" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
@@ -1109,86 +1192,93 @@
     </row>
     <row r="5" spans="1:2" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="24"/>
-    </row>
-    <row r="6" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="32"/>
-    </row>
-    <row r="7" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="27"/>
-    </row>
-    <row r="8" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+    </row>
+    <row r="8" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="25"/>
-    </row>
-    <row r="9" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="25"/>
-    </row>
-    <row r="10" spans="1:2" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="B9" s="24"/>
+    </row>
+    <row r="10" spans="1:2" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25"/>
+    </row>
+    <row r="11" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="26"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="B11" s="26"/>
+    </row>
+    <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="27"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="29"/>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="24"/>
+    </row>
+    <row r="14" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="26"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="27"/>
-    </row>
-    <row r="15" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="B15" s="26"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="27"/>
-    </row>
-    <row r="16" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"?, Atomistic - Class I, Atomistic - Class II, Atomistic - Bond Order, Atomistic - ReaxFF, Atomistic - Polarizable, Atomistic - United Atom (UA), Coarse-Grained (CG) - Pseudo-Atom"</formula1>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{9417C49F-CEF4-4F35-A22F-0A4A8EC2B51D}">
+      <formula1>"Mixed-English,Mixed-Metric,Reduced"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{CA8574A2-2C56-4FA8-AE4A-9714A1E7A46C}">
-      <formula1>"Mixed-English,Mixed-Metric,Reduced"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{4CF6801F-C755-4D4C-A6CE-559B59F1FFB7}">
+      <formula1>"?, Atomistic - Class I, Atomistic - Class II, Atomistic - Water Model, Coarse-Grained"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{8C0FF906-BE83-41D0-9362-07E2219B48AA}">
+      <formula1>"1.0.0"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1216,17 +1306,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="35"/>
+      <c r="A1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5"/>
     </row>
@@ -1236,10 +1326,10 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1382,367 +1472,367 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1751,13 +1841,194 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6031D16A-213F-4BCB-AB57-4F738396A00F}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="41" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="24"/>
+    </row>
+    <row r="7" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="24"/>
+    </row>
+    <row r="13" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
@@ -1771,21 +2042,21 @@
     <col min="7" max="7" width="36.140625" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="29"/>
+    <col min="10" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1800,11 +2071,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1815,10 +2086,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -1831,12 +2102,12 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>18</v>
+      <c r="A5" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1846,12 +2117,12 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>17</v>
+      <c r="A6" s="32" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1862,10 +2133,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -1879,10 +2150,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -1896,10 +2167,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -1913,10 +2184,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -1930,10 +2201,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -1947,10 +2218,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1975,31 +2246,31 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="H14" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="I14" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2037,7 +2308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA409BC-7E78-4597-8B05-CA0A4A659430}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
@@ -2058,21 +2329,21 @@
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="29"/>
+    <col min="10" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2087,11 +2358,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2102,10 +2373,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
@@ -2118,12 +2389,12 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>18</v>
+      <c r="A5" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2133,12 +2404,12 @@
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>17</v>
+      <c r="A6" s="32" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2149,10 +2420,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -2166,10 +2437,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -2183,10 +2454,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -2200,10 +2471,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -2217,10 +2488,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -2234,10 +2505,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -2262,31 +2533,31 @@
     </row>
     <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="H14" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>114</v>
-      </c>
       <c r="I14" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6173248F-86A5-4F55-B24D-4513AEE2F317}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
@@ -2345,24 +2616,24 @@
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="29"/>
+    <col min="13" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2380,11 +2651,11 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2398,10 +2669,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
@@ -2417,12 +2688,12 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>18</v>
+      <c r="A5" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2435,12 +2706,12 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>17</v>
+      <c r="A6" s="32" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2454,10 +2725,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
@@ -2474,10 +2745,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
@@ -2494,10 +2765,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -2514,10 +2785,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -2534,10 +2805,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -2554,10 +2825,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -2588,40 +2859,40 @@
     </row>
     <row r="14" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="F14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="H14" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="K14" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>114</v>
-      </c>
       <c r="L14" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added spreadsheets for flexible models
</commit_message>
<xml_diff>
--- a/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
+++ b/XML/Water-Models/WebFF-WaterModel-DataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Water-Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72039C4-F4BD-47C8-9C53-26D672D1532F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE191517-7F1A-435C-83C8-AA8C73FBA7BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="18195" windowHeight="8190" firstSheet="11" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="40" r:id="rId1"/>
@@ -20,6 +20,16 @@
     <sheet name="WaterModel-3Site-Rigid" sheetId="1" r:id="rId5"/>
     <sheet name="WaterModel-4Site-Rigid" sheetId="37" r:id="rId6"/>
     <sheet name="WaterModel-5Site-Rigid" sheetId="38" r:id="rId7"/>
+    <sheet name="AtomType-ATDL" sheetId="41" r:id="rId8"/>
+    <sheet name="AtomType-Generic" sheetId="43" r:id="rId9"/>
+    <sheet name="BondPotential-Harmonic" sheetId="42" r:id="rId10"/>
+    <sheet name="BondPotential-Morse" sheetId="50" r:id="rId11"/>
+    <sheet name="AnglePotential-Harmonic" sheetId="44" r:id="rId12"/>
+    <sheet name="AnglePotential-COS2" sheetId="45" r:id="rId13"/>
+    <sheet name="NonBondPotential-LJ" sheetId="46" r:id="rId14"/>
+    <sheet name="NonBondPotential-LJ2" sheetId="47" r:id="rId15"/>
+    <sheet name="NonBondPotential-LJ-AB" sheetId="48" r:id="rId16"/>
+    <sheet name="BondIncrements" sheetId="49" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -42,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="190">
   <si>
     <t># Preset</t>
   </si>
@@ -444,13 +454,184 @@
   </si>
   <si>
     <t>Force-Field Protocol</t>
+  </si>
+  <si>
+    <t>Atom-Types</t>
+  </si>
+  <si>
+    <t>Nomenclature</t>
+  </si>
+  <si>
+    <t>ATDL</t>
+  </si>
+  <si>
+    <t># Enter data</t>
+  </si>
+  <si>
+    <t>AtomType-Name</t>
+  </si>
+  <si>
+    <t>Atom</t>
+  </si>
+  <si>
+    <t>BondedAtoms</t>
+  </si>
+  <si>
+    <t>FormalCharge</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>AtomicNumber</t>
+  </si>
+  <si>
+    <t>AtomicMass</t>
+  </si>
+  <si>
+    <t>Bond Potential</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>Harmonic</t>
+  </si>
+  <si>
+    <t>K*(R-R0)^2</t>
+  </si>
+  <si>
+    <t>K-units</t>
+  </si>
+  <si>
+    <t>kJ/mol/nm^2</t>
+  </si>
+  <si>
+    <t>R0-units</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>AT-1</t>
+  </si>
+  <si>
+    <t>AT-2</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>BondPattern</t>
+  </si>
+  <si>
+    <t>Angle Potential</t>
+  </si>
+  <si>
+    <t>Ka*(Theta-Theta0)^2</t>
+  </si>
+  <si>
+    <t>Ka-units</t>
+  </si>
+  <si>
+    <t>kJ/mol/degrees^2</t>
+  </si>
+  <si>
+    <t>Theta0-units</t>
+  </si>
+  <si>
+    <t>AT-3</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>Theta0</t>
+  </si>
+  <si>
+    <t>precedence</t>
+  </si>
+  <si>
+    <t>cosine/squared</t>
+  </si>
+  <si>
+    <t>Ka*[cos(Theta)-cos(Theta0)]^2</t>
+  </si>
+  <si>
+    <t>Non-Bond Potential</t>
+  </si>
+  <si>
+    <t>Lennard-Jones (12-6)</t>
+  </si>
+  <si>
+    <t>4*epsilon*[(sigma/R)^12-(sigma/R)^6]</t>
+  </si>
+  <si>
+    <t>Combining-Rule</t>
+  </si>
+  <si>
+    <t>Kong</t>
+  </si>
+  <si>
+    <t>AtomType</t>
+  </si>
+  <si>
+    <t>Lorentz-Berthelot</t>
+  </si>
+  <si>
+    <t>Lennard-Jones (12-6) [A-B Form]</t>
+  </si>
+  <si>
+    <t>A/(R^12)-B/(R^6)</t>
+  </si>
+  <si>
+    <t>Bond Increments</t>
+  </si>
+  <si>
+    <t>AT-I</t>
+  </si>
+  <si>
+    <t>AT-J</t>
+  </si>
+  <si>
+    <t>Delta-IJ</t>
+  </si>
+  <si>
+    <t>Delta-JI</t>
+  </si>
+  <si>
+    <t>Morse</t>
+  </si>
+  <si>
+    <t>D*[(1-exp(-A(R-R0))]^2</t>
+  </si>
+  <si>
+    <t>D-units</t>
+  </si>
+  <si>
+    <t>1/nm</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,8 +692,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +741,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.24994659260841701"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -703,15 +910,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -774,18 +983,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -807,9 +1004,47 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="7" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent5" xfId="7" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="6" builtinId="31"/>
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -1159,7 +1394,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1171,10 +1406,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1194,7 +1429,7 @@
       <c r="A5" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="40" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1283,6 +1518,3846 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F1677C-B920-4757-9C5A-B63453CB37DB}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{3D8DDFAF-BDB5-4C69-916B-FC2D5899F0A7}">
+      <formula1>"Harmonic"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{20BF28C8-965F-487A-8906-F06B799EF466}">
+      <formula1>"K*(R-R0)^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{B695E6CC-3EDA-44B9-990A-18423D8D896B}">
+      <formula1>"?, kcal/mol/Å^2, kJ/mol/nm^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{890391E1-3DD4-40B3-9C4E-1DBA6F9579A2}">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D03A6FD-943B-479E-BEAE-5EEECA7E4B62}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{E174DB35-33A5-4301-9BDD-2402C5DBA7DC}">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{2C59073E-DE1C-4D4A-B44A-349AC90001A2}">
+      <formula1>"Morse"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{B07748AE-CD6D-42E1-83D6-3164EB464735}">
+      <formula1>"D*[(1-exp(-A(R-R0))]^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{CFA3939E-0A5B-4D05-BA40-9E4BB112452D}">
+      <formula1>"? , kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{2E746FBF-15DC-4139-BFC1-2EDAE18C2716}">
+      <formula1>"?, 1/Å, 1/nm"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A3C936-69F4-4484-8223-99F25E21BE39}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{ADE4C20C-F580-4916-8B69-AE2EC48BCE5E}">
+      <formula1>"degrees"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{001A45B6-BE7A-48A8-AEAF-2B469BEB0944}">
+      <formula1>"?, kcal/mol/degrees^2, kJ/mol/degrees^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{1B8DE41F-568F-4EE3-BF85-7DBC7C81D9AB}">
+      <formula1>"Ka*(Theta-Theta0)^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{F1AE9AFE-346B-4AF9-9D95-78C7A298159B}">
+      <formula1>"Harmonic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387109B9-849D-4665-B6BE-63FAA8C6E33A}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="51"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{F03CC5ED-0FB2-48CF-87B1-7B7A109ECCF3}">
+      <formula1>"cosine/squared"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{8825EC90-22B6-4E13-A7CC-26A06E2CCC52}">
+      <formula1>"Ka*[cos(Theta)-cos(Theta0)]^2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{E401B4AE-BFD7-4EEF-BAF2-01BD72BA712D}">
+      <formula1>"?,kcal/mol,kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{4CA5A016-10F0-4389-9A29-C4E587E12E32}">
+      <formula1>"degrees"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC927D7-2D33-4F9A-8D8D-3594726EBA94}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{7B58391B-32F5-4BFC-9955-BFEABCE3CF2A}">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{4FBD4899-2BB7-4892-8A3A-2A7768D04353}">
+      <formula1>"?, kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{59562904-54C9-44F6-A101-E81D2EB7ECF9}">
+      <formula1>"4*epsilon*[(sigma/R)^12-(sigma/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{C494EB8E-5F47-4FDE-9B1C-AF5BDAA48BD1}">
+      <formula1>"Lennard-Jones (12-6)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{AA629BB5-A9FF-4B2B-ACE5-00AD799BF4E8}">
+      <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B4C85E-5991-4BA4-96F8-1A359F3D2342}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{B8FB8F08-CD51-4815-93D0-9319F00C298C}">
+      <formula1>"?,Lorentz-Berthelot,Waldman-Hagler,Kong,Fender-Halsey"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{79FD0E95-AD50-42C0-9BDB-CACD5D3AE5B2}">
+      <formula1>"Lennard-Jones (12-6)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{689B9C83-61F9-46AD-B7F7-FFBBF8EEEE91}">
+      <formula1>"4*epsilon*[(sigma/R)^12-(sigma/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{831631AF-07CF-44C3-997D-38B5E54AF90C}">
+      <formula1>"?, kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{A100928A-35BD-4C69-B493-E3685B0D85E3}">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777653BE-8C16-40B8-8FDE-1F8C0A2CB41E}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:G711"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="F10" s="55"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="F11" s="55"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="F15" s="55"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="F16" s="55"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="F17" s="55"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="F18" s="55"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="F19" s="55"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="F20" s="55"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="F21" s="55"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="F22" s="55"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="F23" s="55"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="F24" s="55"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="F25" s="55"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="F26" s="55"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="F27" s="55"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="F28" s="55"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="F29" s="55"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="F30" s="55"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="F31" s="55"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="F32" s="55"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="F33" s="55"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="F34" s="55"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="F35" s="55"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="F36" s="55"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="F37" s="55"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="F38" s="55"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="F39" s="55"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="F41" s="55"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="F42" s="55"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="F43" s="55"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="F44" s="55"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="F45" s="55"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="F46" s="55"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="F47" s="55"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="F48" s="55"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="F49" s="55"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="F50" s="55"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="F51" s="55"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="F52" s="55"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="F53" s="55"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="F54" s="55"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="F55" s="55"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="F56" s="55"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="F57" s="55"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+      <c r="F58" s="55"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+      <c r="F59" s="55"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+      <c r="F60" s="55"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="F61" s="55"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="F62" s="55"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+      <c r="F63" s="55"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="F64" s="55"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="F65" s="55"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="F66" s="55"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="F67" s="55"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+      <c r="F68" s="55"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="F69" s="55"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="F70" s="55"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="F71" s="55"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="F72" s="55"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+      <c r="F73" s="55"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+      <c r="F74" s="55"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+      <c r="F75" s="55"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="F76" s="55"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+      <c r="F77" s="55"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+      <c r="F78" s="55"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+      <c r="F79" s="55"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+      <c r="F80" s="55"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+      <c r="F81" s="55"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82"/>
+      <c r="F82" s="55"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+      <c r="F83" s="55"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+      <c r="F84" s="55"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="F85" s="55"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="F86" s="55"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="F87" s="55"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="F88" s="55"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="F89" s="55"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="F90" s="55"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="F91" s="55"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="F92" s="55"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="F93" s="55"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="F94" s="55"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="F95" s="55"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+      <c r="F96" s="55"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+      <c r="F97" s="55"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+      <c r="F98" s="55"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99"/>
+      <c r="F99" s="55"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100"/>
+      <c r="F100" s="55"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101"/>
+      <c r="F101" s="55"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102"/>
+      <c r="F102" s="55"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103"/>
+      <c r="F103" s="55"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104"/>
+      <c r="F104" s="55"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105"/>
+      <c r="F105" s="55"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106"/>
+      <c r="F106" s="55"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107"/>
+      <c r="F107" s="55"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108"/>
+      <c r="F108" s="55"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109"/>
+      <c r="F109" s="55"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110"/>
+      <c r="F110" s="55"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111"/>
+      <c r="F111" s="55"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112"/>
+      <c r="F112" s="55"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+      <c r="F113" s="55"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114"/>
+      <c r="F114" s="55"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115"/>
+      <c r="F115" s="55"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116"/>
+      <c r="F116" s="55"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117"/>
+      <c r="F117" s="55"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118"/>
+      <c r="F118" s="55"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119"/>
+      <c r="F119" s="55"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120"/>
+      <c r="F120" s="55"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121"/>
+      <c r="F121" s="55"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122"/>
+      <c r="F122" s="55"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123"/>
+      <c r="F123" s="55"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124"/>
+      <c r="F124" s="55"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125"/>
+      <c r="F125" s="55"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126"/>
+      <c r="F126" s="55"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127"/>
+      <c r="F127" s="55"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128"/>
+      <c r="F128" s="55"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129"/>
+      <c r="F129" s="55"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130"/>
+      <c r="F130" s="55"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131"/>
+      <c r="F131" s="55"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132"/>
+      <c r="F132" s="55"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133"/>
+      <c r="F133" s="55"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134"/>
+      <c r="F134" s="55"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135"/>
+      <c r="F135" s="55"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136"/>
+      <c r="F136" s="55"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137"/>
+      <c r="F137" s="55"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138"/>
+      <c r="F138" s="55"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139"/>
+      <c r="F139" s="55"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140"/>
+      <c r="F140" s="55"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141"/>
+      <c r="F141" s="55"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142"/>
+      <c r="F142" s="55"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143"/>
+      <c r="F143" s="55"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144"/>
+      <c r="F144" s="55"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145"/>
+      <c r="F145" s="55"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146"/>
+      <c r="F146" s="55"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147"/>
+      <c r="F147" s="55"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148"/>
+      <c r="F148" s="55"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149"/>
+      <c r="F149" s="55"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150"/>
+      <c r="F150" s="55"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151"/>
+      <c r="F151" s="55"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152"/>
+      <c r="F152" s="55"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153"/>
+      <c r="F153" s="55"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154"/>
+      <c r="F154" s="55"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155"/>
+      <c r="F155" s="55"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156"/>
+      <c r="F156" s="55"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157"/>
+      <c r="F157" s="55"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158"/>
+      <c r="F158" s="55"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159"/>
+      <c r="F159" s="55"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160"/>
+      <c r="F160" s="55"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161"/>
+      <c r="F161" s="55"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162"/>
+      <c r="F162" s="55"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163"/>
+      <c r="F163" s="55"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164"/>
+      <c r="F164" s="55"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165"/>
+      <c r="F165" s="55"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166"/>
+      <c r="F166" s="55"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167"/>
+      <c r="F167" s="55"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168"/>
+      <c r="F168" s="55"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169"/>
+      <c r="F169" s="55"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170"/>
+      <c r="F170" s="55"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171"/>
+      <c r="F171" s="55"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172"/>
+      <c r="F172" s="55"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173"/>
+      <c r="F173" s="55"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174"/>
+      <c r="F174" s="55"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175"/>
+      <c r="F175" s="55"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176"/>
+      <c r="F176" s="55"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177"/>
+      <c r="F177" s="55"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178"/>
+      <c r="F178" s="55"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179"/>
+      <c r="F179" s="55"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180"/>
+      <c r="F180" s="55"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181"/>
+      <c r="F181" s="55"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182"/>
+      <c r="F182" s="55"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183"/>
+      <c r="F183" s="55"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184"/>
+      <c r="F184" s="55"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185"/>
+      <c r="F185" s="55"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186"/>
+      <c r="F186" s="55"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187"/>
+      <c r="F187" s="55"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188"/>
+      <c r="F188" s="55"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189"/>
+      <c r="F189" s="55"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190"/>
+      <c r="F190" s="55"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191"/>
+      <c r="F191" s="55"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192"/>
+      <c r="F192" s="55"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193"/>
+      <c r="F193" s="55"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194"/>
+      <c r="F194" s="55"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195"/>
+      <c r="F195" s="55"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196"/>
+      <c r="F196" s="55"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197"/>
+      <c r="F197" s="55"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198"/>
+      <c r="F198" s="55"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199"/>
+      <c r="F199" s="55"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200"/>
+      <c r="F200" s="55"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201"/>
+      <c r="F201" s="55"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202"/>
+      <c r="F202" s="55"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203"/>
+      <c r="F203" s="55"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204"/>
+      <c r="F204" s="55"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205"/>
+      <c r="F205" s="55"/>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206"/>
+      <c r="F206" s="55"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207"/>
+      <c r="F207" s="55"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208"/>
+      <c r="F208" s="55"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209"/>
+      <c r="F209" s="55"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210"/>
+      <c r="F210" s="55"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211"/>
+      <c r="F211" s="55"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212"/>
+      <c r="F212" s="55"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213"/>
+      <c r="F213" s="55"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214"/>
+      <c r="F214" s="55"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215"/>
+      <c r="F215" s="55"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216"/>
+      <c r="F216" s="55"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217"/>
+      <c r="F217" s="55"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218"/>
+      <c r="F218" s="55"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219"/>
+      <c r="F219" s="55"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220"/>
+      <c r="F220" s="55"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221"/>
+      <c r="F221" s="55"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222"/>
+      <c r="F222" s="55"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223"/>
+      <c r="F223" s="55"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224"/>
+      <c r="F224" s="55"/>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225"/>
+      <c r="F225" s="55"/>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226"/>
+      <c r="F226" s="55"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227"/>
+      <c r="F227" s="55"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228"/>
+      <c r="F228" s="55"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229"/>
+      <c r="F229" s="55"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230"/>
+      <c r="F230" s="55"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231"/>
+      <c r="F231" s="55"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232"/>
+      <c r="F232" s="55"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233"/>
+      <c r="F233" s="55"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234"/>
+      <c r="F234" s="55"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235"/>
+      <c r="F235" s="55"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236"/>
+      <c r="F236" s="55"/>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237"/>
+      <c r="F237" s="55"/>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238"/>
+      <c r="F238" s="55"/>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239"/>
+      <c r="F239" s="55"/>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240"/>
+      <c r="F240" s="55"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241"/>
+      <c r="F241" s="55"/>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242"/>
+      <c r="F242" s="55"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243"/>
+      <c r="F243" s="55"/>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244"/>
+      <c r="F244" s="55"/>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245"/>
+      <c r="F245" s="55"/>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246"/>
+      <c r="F246" s="55"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247"/>
+      <c r="F247" s="55"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248"/>
+      <c r="F248" s="55"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249"/>
+      <c r="F249" s="55"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250"/>
+      <c r="F250" s="55"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251"/>
+      <c r="F251" s="55"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252"/>
+      <c r="F252" s="55"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253"/>
+      <c r="F253" s="55"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254"/>
+      <c r="F254" s="55"/>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255"/>
+      <c r="F255" s="55"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256"/>
+      <c r="F256" s="55"/>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257"/>
+      <c r="F257" s="55"/>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258"/>
+      <c r="F258" s="55"/>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259"/>
+      <c r="F259" s="55"/>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260"/>
+      <c r="F260" s="55"/>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261"/>
+      <c r="F261" s="55"/>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262"/>
+      <c r="F262" s="55"/>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263"/>
+      <c r="F263" s="55"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264"/>
+      <c r="F264" s="55"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265"/>
+      <c r="F265" s="55"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266"/>
+      <c r="F266" s="55"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267"/>
+      <c r="F267" s="55"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268"/>
+      <c r="F268" s="55"/>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269"/>
+      <c r="F269" s="55"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270"/>
+      <c r="F270" s="55"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271"/>
+      <c r="F271" s="55"/>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272"/>
+      <c r="F272" s="55"/>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273"/>
+      <c r="F273" s="55"/>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274"/>
+      <c r="F274" s="55"/>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275"/>
+      <c r="F275" s="55"/>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276"/>
+      <c r="F276" s="55"/>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277"/>
+      <c r="F277" s="55"/>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278"/>
+      <c r="F278" s="55"/>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279"/>
+      <c r="F279" s="55"/>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280"/>
+      <c r="F280" s="55"/>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281"/>
+      <c r="F281" s="55"/>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282"/>
+      <c r="F282" s="55"/>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283"/>
+      <c r="F283" s="55"/>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284"/>
+      <c r="F284" s="55"/>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285"/>
+      <c r="F285" s="55"/>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286"/>
+      <c r="F286" s="55"/>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287"/>
+      <c r="F287" s="55"/>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288"/>
+      <c r="F288" s="55"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289"/>
+      <c r="F289" s="55"/>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290"/>
+      <c r="F290" s="55"/>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291"/>
+      <c r="F291" s="55"/>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292"/>
+      <c r="F292" s="55"/>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293"/>
+      <c r="F293" s="55"/>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294"/>
+      <c r="F294" s="55"/>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295"/>
+      <c r="F295" s="55"/>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296"/>
+      <c r="F296" s="55"/>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297"/>
+      <c r="F297" s="55"/>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298"/>
+      <c r="F298" s="55"/>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299"/>
+      <c r="F299" s="55"/>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300"/>
+      <c r="F300" s="55"/>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301"/>
+      <c r="F301" s="55"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302"/>
+      <c r="F302" s="55"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303"/>
+      <c r="F303" s="55"/>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304"/>
+      <c r="F304" s="55"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305"/>
+      <c r="F305" s="55"/>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306"/>
+      <c r="F306" s="55"/>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307"/>
+      <c r="F307" s="55"/>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308"/>
+      <c r="F308" s="55"/>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309"/>
+      <c r="F309" s="55"/>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310"/>
+      <c r="F310" s="55"/>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311"/>
+      <c r="F311" s="55"/>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312"/>
+      <c r="F312" s="55"/>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313"/>
+      <c r="F313" s="55"/>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314"/>
+      <c r="F314" s="55"/>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315"/>
+      <c r="F315" s="55"/>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316"/>
+      <c r="F316" s="55"/>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317"/>
+      <c r="F317" s="55"/>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318"/>
+      <c r="F318" s="55"/>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319"/>
+      <c r="F319" s="55"/>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320"/>
+      <c r="F320" s="55"/>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321"/>
+      <c r="F321" s="55"/>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322"/>
+      <c r="F322" s="55"/>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323"/>
+      <c r="F323" s="55"/>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324"/>
+      <c r="F324" s="55"/>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325"/>
+      <c r="F325" s="55"/>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326"/>
+      <c r="F326" s="55"/>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327"/>
+      <c r="F327" s="55"/>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328"/>
+      <c r="F328" s="55"/>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329"/>
+      <c r="F329" s="55"/>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330"/>
+      <c r="F330" s="55"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331"/>
+      <c r="F331" s="55"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332"/>
+      <c r="F332" s="55"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333"/>
+      <c r="F333" s="55"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334"/>
+      <c r="F334" s="55"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335"/>
+      <c r="F335" s="55"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336"/>
+      <c r="F336" s="55"/>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337"/>
+      <c r="F337" s="55"/>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338"/>
+      <c r="F338" s="55"/>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339"/>
+      <c r="F339" s="55"/>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340"/>
+      <c r="F340" s="55"/>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341"/>
+      <c r="F341" s="55"/>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342"/>
+      <c r="F342" s="55"/>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343"/>
+      <c r="F343" s="55"/>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344"/>
+      <c r="F344" s="55"/>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345"/>
+      <c r="F345" s="55"/>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346"/>
+      <c r="F346" s="55"/>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347"/>
+      <c r="F347" s="55"/>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348"/>
+      <c r="F348" s="55"/>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349"/>
+      <c r="F349" s="55"/>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350"/>
+      <c r="F350" s="55"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351"/>
+      <c r="F351" s="55"/>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352"/>
+      <c r="F352" s="55"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353"/>
+      <c r="F353" s="55"/>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354"/>
+      <c r="F354" s="55"/>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355"/>
+      <c r="F355" s="55"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356"/>
+      <c r="F356" s="55"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357"/>
+      <c r="F357" s="55"/>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358"/>
+      <c r="F358" s="55"/>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359"/>
+      <c r="F359" s="55"/>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360"/>
+      <c r="F360" s="55"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361"/>
+      <c r="F361" s="55"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362"/>
+      <c r="F362" s="55"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363"/>
+      <c r="F363" s="55"/>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364"/>
+      <c r="F364" s="55"/>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365"/>
+      <c r="F365" s="55"/>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366"/>
+      <c r="F366" s="55"/>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367"/>
+      <c r="F367" s="55"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368"/>
+      <c r="F368" s="55"/>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369"/>
+      <c r="F369" s="55"/>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370"/>
+      <c r="F370" s="55"/>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371"/>
+      <c r="F371" s="55"/>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372"/>
+      <c r="F372" s="55"/>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373"/>
+      <c r="F373" s="55"/>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374"/>
+      <c r="F374" s="55"/>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375"/>
+      <c r="F375" s="55"/>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376"/>
+      <c r="F376" s="55"/>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377"/>
+      <c r="F377" s="55"/>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378"/>
+      <c r="F378" s="55"/>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379"/>
+      <c r="F379" s="55"/>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380"/>
+      <c r="F380" s="55"/>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381"/>
+      <c r="F381" s="55"/>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382"/>
+      <c r="F382" s="55"/>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383"/>
+      <c r="F383" s="55"/>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384"/>
+      <c r="F384" s="55"/>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385"/>
+      <c r="F385" s="55"/>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386"/>
+      <c r="F386" s="55"/>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387"/>
+      <c r="F387" s="55"/>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388"/>
+      <c r="F388" s="55"/>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389"/>
+      <c r="F389" s="55"/>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390"/>
+      <c r="F390" s="55"/>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391"/>
+      <c r="F391" s="55"/>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392"/>
+      <c r="F392" s="55"/>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393"/>
+      <c r="F393" s="55"/>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394"/>
+      <c r="F394" s="55"/>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395"/>
+      <c r="F395" s="55"/>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396"/>
+      <c r="F396" s="55"/>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397"/>
+      <c r="F397" s="55"/>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398"/>
+      <c r="F398" s="55"/>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399"/>
+      <c r="F399" s="55"/>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400"/>
+      <c r="F400" s="55"/>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401"/>
+      <c r="F401" s="55"/>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402"/>
+      <c r="F402" s="55"/>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403"/>
+      <c r="F403" s="55"/>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404"/>
+      <c r="F404" s="55"/>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405"/>
+      <c r="F405" s="55"/>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A406"/>
+      <c r="F406" s="55"/>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A407"/>
+      <c r="F407" s="55"/>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A408"/>
+      <c r="F408" s="55"/>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A409"/>
+      <c r="F409" s="55"/>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A410"/>
+      <c r="F410" s="55"/>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411"/>
+      <c r="F411" s="55"/>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A412"/>
+      <c r="F412" s="55"/>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A413"/>
+      <c r="F413" s="55"/>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A414"/>
+      <c r="F414" s="55"/>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A415"/>
+      <c r="F415" s="55"/>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A416"/>
+      <c r="F416" s="55"/>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A417"/>
+      <c r="F417" s="55"/>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A418"/>
+      <c r="F418" s="55"/>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A419"/>
+      <c r="F419" s="55"/>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A420"/>
+      <c r="F420" s="55"/>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421"/>
+      <c r="F421" s="55"/>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A422"/>
+      <c r="F422" s="55"/>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423"/>
+      <c r="F423" s="55"/>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424"/>
+      <c r="F424" s="55"/>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425"/>
+      <c r="F425" s="55"/>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426"/>
+      <c r="F426" s="55"/>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427"/>
+      <c r="F427" s="55"/>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428"/>
+      <c r="F428" s="55"/>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A429"/>
+      <c r="F429" s="55"/>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A430"/>
+      <c r="F430" s="55"/>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A431"/>
+      <c r="F431" s="55"/>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A432"/>
+      <c r="F432" s="55"/>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433"/>
+      <c r="F433" s="55"/>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434"/>
+      <c r="F434" s="55"/>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435"/>
+      <c r="F435" s="55"/>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436"/>
+      <c r="F436" s="55"/>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437"/>
+      <c r="F437" s="55"/>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438"/>
+      <c r="F438" s="55"/>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439"/>
+      <c r="F439" s="55"/>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440"/>
+      <c r="F440" s="55"/>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441"/>
+      <c r="F441" s="55"/>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442"/>
+      <c r="F442" s="55"/>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443"/>
+      <c r="F443" s="55"/>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444"/>
+      <c r="F444" s="55"/>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445"/>
+      <c r="F445" s="55"/>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446"/>
+      <c r="F446" s="55"/>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447"/>
+      <c r="F447" s="55"/>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448"/>
+      <c r="F448" s="55"/>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449"/>
+      <c r="F449" s="55"/>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A450"/>
+      <c r="F450" s="55"/>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A451"/>
+      <c r="F451" s="55"/>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A452"/>
+      <c r="F452" s="55"/>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A453"/>
+      <c r="F453" s="55"/>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A454"/>
+      <c r="F454" s="55"/>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A455"/>
+      <c r="F455" s="55"/>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A456"/>
+      <c r="F456" s="55"/>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457"/>
+      <c r="F457" s="55"/>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458"/>
+      <c r="F458" s="55"/>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459"/>
+      <c r="F459" s="55"/>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460"/>
+      <c r="F460" s="55"/>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A461"/>
+      <c r="F461" s="55"/>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462"/>
+      <c r="F462" s="55"/>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463"/>
+      <c r="F463" s="55"/>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A464"/>
+      <c r="F464" s="55"/>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465"/>
+      <c r="F465" s="55"/>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466"/>
+      <c r="F466" s="55"/>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A467"/>
+      <c r="F467" s="55"/>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468"/>
+      <c r="F468" s="55"/>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469"/>
+      <c r="F469" s="55"/>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470"/>
+      <c r="F470" s="55"/>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471"/>
+      <c r="F471" s="55"/>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472"/>
+      <c r="F472" s="55"/>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473"/>
+      <c r="F473" s="55"/>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474"/>
+      <c r="F474" s="55"/>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475"/>
+      <c r="F475" s="55"/>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476"/>
+      <c r="F476" s="55"/>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477"/>
+      <c r="F477" s="55"/>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478"/>
+      <c r="F478" s="55"/>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479"/>
+      <c r="F479" s="55"/>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480"/>
+      <c r="F480" s="55"/>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481"/>
+      <c r="F481" s="55"/>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482"/>
+      <c r="F482" s="55"/>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483"/>
+      <c r="F483" s="55"/>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484"/>
+      <c r="F484" s="55"/>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485"/>
+      <c r="F485" s="55"/>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486"/>
+      <c r="F486" s="55"/>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487"/>
+      <c r="F487" s="55"/>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488"/>
+      <c r="F488" s="55"/>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489"/>
+      <c r="F489" s="55"/>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490"/>
+      <c r="F490" s="55"/>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491"/>
+      <c r="F491" s="55"/>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492"/>
+      <c r="F492" s="55"/>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493"/>
+      <c r="F493" s="55"/>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494"/>
+      <c r="F494" s="55"/>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495"/>
+      <c r="F495" s="55"/>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496"/>
+      <c r="F496" s="55"/>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497"/>
+      <c r="F497" s="55"/>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498"/>
+      <c r="F498" s="55"/>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499"/>
+      <c r="F499" s="55"/>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500"/>
+      <c r="F500" s="55"/>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501"/>
+      <c r="F501" s="55"/>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502"/>
+      <c r="F502" s="55"/>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503"/>
+      <c r="F503" s="55"/>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504"/>
+      <c r="F504" s="55"/>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505"/>
+      <c r="F505" s="55"/>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506"/>
+      <c r="F506" s="55"/>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507"/>
+      <c r="F507" s="55"/>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508"/>
+      <c r="F508" s="55"/>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509"/>
+      <c r="F509" s="55"/>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510"/>
+      <c r="F510" s="55"/>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511"/>
+      <c r="F511" s="55"/>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512"/>
+      <c r="F512" s="55"/>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513"/>
+      <c r="F513" s="55"/>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514"/>
+      <c r="F514" s="55"/>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515"/>
+      <c r="F515" s="55"/>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516"/>
+      <c r="F516" s="55"/>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517"/>
+      <c r="F517" s="55"/>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518"/>
+      <c r="F518" s="55"/>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519"/>
+      <c r="F519" s="55"/>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520"/>
+      <c r="F520" s="55"/>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521"/>
+      <c r="F521" s="55"/>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522"/>
+      <c r="F522" s="55"/>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523"/>
+      <c r="F523" s="55"/>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524"/>
+      <c r="F524" s="55"/>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525"/>
+      <c r="F525" s="55"/>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526"/>
+      <c r="F526" s="55"/>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527"/>
+      <c r="F527" s="55"/>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528"/>
+      <c r="F528" s="55"/>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529"/>
+      <c r="F529" s="55"/>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530"/>
+      <c r="F530" s="55"/>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531"/>
+      <c r="F531" s="55"/>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532"/>
+      <c r="F532" s="55"/>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533"/>
+      <c r="F533" s="55"/>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534"/>
+      <c r="F534" s="55"/>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535"/>
+      <c r="F535" s="55"/>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536"/>
+      <c r="F536" s="55"/>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537"/>
+      <c r="F537" s="55"/>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A538"/>
+      <c r="F538" s="55"/>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A539"/>
+      <c r="F539" s="55"/>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A540"/>
+      <c r="F540" s="55"/>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A541"/>
+      <c r="F541" s="55"/>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542"/>
+      <c r="F542" s="55"/>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A543"/>
+      <c r="F543" s="55"/>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A544"/>
+      <c r="F544" s="55"/>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A545"/>
+      <c r="F545" s="55"/>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A546"/>
+      <c r="F546" s="55"/>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A547"/>
+      <c r="F547" s="55"/>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548"/>
+      <c r="F548" s="55"/>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549"/>
+      <c r="F549" s="55"/>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550"/>
+      <c r="F550" s="55"/>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551"/>
+      <c r="F551" s="55"/>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552"/>
+      <c r="F552" s="55"/>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553"/>
+      <c r="F553" s="55"/>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554"/>
+      <c r="F554" s="55"/>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555"/>
+      <c r="F555" s="55"/>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556"/>
+      <c r="F556" s="55"/>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557"/>
+      <c r="F557" s="55"/>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558"/>
+      <c r="F558" s="55"/>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559"/>
+      <c r="F559" s="55"/>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560"/>
+      <c r="F560" s="55"/>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561"/>
+      <c r="F561" s="55"/>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562"/>
+      <c r="F562" s="55"/>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563"/>
+      <c r="F563" s="55"/>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564"/>
+      <c r="F564" s="55"/>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565"/>
+      <c r="F565" s="55"/>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566"/>
+      <c r="F566" s="55"/>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A567"/>
+      <c r="F567" s="55"/>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A568"/>
+      <c r="F568" s="55"/>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A569"/>
+      <c r="F569" s="55"/>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A570"/>
+      <c r="F570" s="55"/>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A571"/>
+      <c r="F571" s="55"/>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A572"/>
+      <c r="F572" s="55"/>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A573"/>
+      <c r="F573" s="55"/>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A574"/>
+      <c r="F574" s="55"/>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A575"/>
+      <c r="F575" s="55"/>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A576"/>
+      <c r="F576" s="55"/>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A577"/>
+      <c r="F577" s="55"/>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A578"/>
+      <c r="F578" s="55"/>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A579"/>
+      <c r="F579" s="55"/>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A580"/>
+      <c r="F580" s="55"/>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A581"/>
+      <c r="F581" s="55"/>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A582"/>
+      <c r="F582" s="55"/>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A583"/>
+      <c r="F583" s="55"/>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A584"/>
+      <c r="F584" s="55"/>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A585"/>
+      <c r="F585" s="55"/>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A586"/>
+      <c r="F586" s="55"/>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A587"/>
+      <c r="F587" s="55"/>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A588"/>
+      <c r="F588" s="55"/>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A589"/>
+      <c r="F589" s="55"/>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A590"/>
+      <c r="F590" s="55"/>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A591"/>
+      <c r="F591" s="55"/>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A592"/>
+      <c r="F592" s="55"/>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A593"/>
+      <c r="F593" s="55"/>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A594"/>
+      <c r="F594" s="55"/>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A595"/>
+      <c r="F595" s="55"/>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A596"/>
+      <c r="F596" s="55"/>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A597"/>
+      <c r="F597" s="55"/>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A598"/>
+      <c r="F598" s="55"/>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A599"/>
+      <c r="F599" s="55"/>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A600"/>
+      <c r="F600" s="55"/>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A601"/>
+      <c r="F601" s="55"/>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A602"/>
+      <c r="F602" s="55"/>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A603"/>
+      <c r="F603" s="55"/>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A604"/>
+      <c r="F604" s="55"/>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A605"/>
+      <c r="F605" s="55"/>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A606"/>
+      <c r="F606" s="55"/>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A607"/>
+      <c r="F607" s="55"/>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A608"/>
+      <c r="F608" s="55"/>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A609"/>
+      <c r="F609" s="55"/>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A610"/>
+      <c r="F610" s="55"/>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A611"/>
+      <c r="F611" s="55"/>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A612"/>
+      <c r="F612" s="55"/>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A613"/>
+      <c r="F613" s="55"/>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A614"/>
+      <c r="F614" s="55"/>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A615"/>
+      <c r="F615" s="55"/>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A616"/>
+      <c r="F616" s="55"/>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A617"/>
+      <c r="F617" s="55"/>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A618"/>
+      <c r="F618" s="55"/>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A619"/>
+      <c r="F619" s="55"/>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A620"/>
+      <c r="F620" s="55"/>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A621"/>
+      <c r="F621" s="55"/>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A622"/>
+      <c r="F622" s="55"/>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A623"/>
+      <c r="F623" s="55"/>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A624"/>
+      <c r="F624" s="55"/>
+    </row>
+    <row r="625" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A625"/>
+      <c r="F625" s="55"/>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A626"/>
+      <c r="F626" s="55"/>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A627"/>
+      <c r="F627" s="55"/>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A628"/>
+      <c r="F628" s="55"/>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A629"/>
+      <c r="F629" s="55"/>
+    </row>
+    <row r="630" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A630"/>
+      <c r="F630" s="55"/>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A631"/>
+      <c r="F631" s="55"/>
+    </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A632"/>
+      <c r="F632" s="55"/>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A633"/>
+      <c r="F633" s="55"/>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A634"/>
+      <c r="F634" s="55"/>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A635"/>
+      <c r="F635" s="55"/>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A636"/>
+      <c r="F636" s="55"/>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A637"/>
+      <c r="F637" s="55"/>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A638"/>
+      <c r="F638" s="55"/>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A639"/>
+      <c r="F639" s="55"/>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A640"/>
+      <c r="F640" s="55"/>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A641"/>
+      <c r="F641" s="55"/>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A642"/>
+      <c r="F642" s="55"/>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A643"/>
+      <c r="F643" s="55"/>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A644"/>
+      <c r="F644" s="55"/>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A645"/>
+      <c r="F645" s="55"/>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A646"/>
+      <c r="F646" s="55"/>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A647"/>
+      <c r="F647" s="55"/>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A648"/>
+      <c r="F648" s="55"/>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A649"/>
+      <c r="F649" s="55"/>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A650"/>
+      <c r="F650" s="55"/>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A651"/>
+      <c r="F651" s="55"/>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A652"/>
+      <c r="F652" s="55"/>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A653"/>
+      <c r="F653" s="55"/>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A654"/>
+      <c r="F654" s="55"/>
+    </row>
+    <row r="655" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A655"/>
+      <c r="F655" s="55"/>
+    </row>
+    <row r="656" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A656"/>
+      <c r="F656" s="55"/>
+    </row>
+    <row r="657" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A657"/>
+      <c r="F657" s="55"/>
+    </row>
+    <row r="658" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A658"/>
+      <c r="F658" s="55"/>
+    </row>
+    <row r="659" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A659"/>
+      <c r="F659" s="55"/>
+    </row>
+    <row r="660" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A660"/>
+      <c r="F660" s="55"/>
+    </row>
+    <row r="661" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A661"/>
+      <c r="F661" s="55"/>
+    </row>
+    <row r="662" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A662"/>
+      <c r="F662" s="55"/>
+    </row>
+    <row r="663" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A663"/>
+      <c r="F663" s="55"/>
+    </row>
+    <row r="664" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A664"/>
+      <c r="F664" s="55"/>
+    </row>
+    <row r="665" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A665"/>
+      <c r="F665" s="55"/>
+    </row>
+    <row r="666" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A666"/>
+      <c r="F666" s="55"/>
+    </row>
+    <row r="667" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A667"/>
+      <c r="F667" s="55"/>
+    </row>
+    <row r="668" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A668"/>
+      <c r="F668" s="55"/>
+    </row>
+    <row r="669" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A669"/>
+      <c r="F669" s="55"/>
+    </row>
+    <row r="670" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A670"/>
+      <c r="F670" s="55"/>
+    </row>
+    <row r="671" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A671"/>
+      <c r="F671" s="55"/>
+    </row>
+    <row r="672" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A672"/>
+      <c r="F672" s="55"/>
+    </row>
+    <row r="673" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A673"/>
+      <c r="F673" s="55"/>
+    </row>
+    <row r="674" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A674"/>
+      <c r="F674" s="55"/>
+    </row>
+    <row r="675" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A675"/>
+      <c r="F675" s="55"/>
+    </row>
+    <row r="676" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A676"/>
+      <c r="F676" s="55"/>
+    </row>
+    <row r="677" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A677"/>
+      <c r="F677" s="55"/>
+    </row>
+    <row r="678" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A678"/>
+      <c r="F678" s="55"/>
+    </row>
+    <row r="679" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A679"/>
+      <c r="F679" s="55"/>
+    </row>
+    <row r="680" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A680"/>
+      <c r="F680" s="55"/>
+    </row>
+    <row r="681" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A681"/>
+      <c r="F681" s="55"/>
+    </row>
+    <row r="682" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A682"/>
+      <c r="F682" s="55"/>
+    </row>
+    <row r="683" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A683"/>
+      <c r="F683" s="55"/>
+    </row>
+    <row r="684" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A684"/>
+      <c r="F684" s="55"/>
+    </row>
+    <row r="685" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A685"/>
+      <c r="F685" s="55"/>
+    </row>
+    <row r="686" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A686"/>
+      <c r="F686" s="55"/>
+    </row>
+    <row r="687" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A687"/>
+      <c r="F687" s="55"/>
+    </row>
+    <row r="688" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A688"/>
+      <c r="F688" s="55"/>
+    </row>
+    <row r="689" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A689"/>
+      <c r="F689" s="55"/>
+    </row>
+    <row r="690" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A690"/>
+      <c r="F690" s="55"/>
+    </row>
+    <row r="691" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A691"/>
+      <c r="F691" s="55"/>
+    </row>
+    <row r="692" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A692"/>
+      <c r="F692" s="55"/>
+    </row>
+    <row r="693" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A693"/>
+      <c r="F693" s="55"/>
+    </row>
+    <row r="694" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A694"/>
+      <c r="F694" s="55"/>
+    </row>
+    <row r="695" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A695"/>
+      <c r="F695" s="55"/>
+    </row>
+    <row r="696" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A696"/>
+      <c r="F696" s="55"/>
+    </row>
+    <row r="697" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A697"/>
+      <c r="F697" s="55"/>
+    </row>
+    <row r="698" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A698"/>
+      <c r="F698" s="55"/>
+    </row>
+    <row r="699" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A699"/>
+      <c r="F699" s="55"/>
+    </row>
+    <row r="700" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A700"/>
+      <c r="F700" s="55"/>
+    </row>
+    <row r="701" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A701"/>
+      <c r="F701" s="55"/>
+    </row>
+    <row r="702" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A702"/>
+      <c r="F702" s="55"/>
+    </row>
+    <row r="703" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A703"/>
+      <c r="F703" s="55"/>
+    </row>
+    <row r="704" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A704"/>
+      <c r="F704" s="55"/>
+    </row>
+    <row r="705" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A705"/>
+      <c r="F705" s="55"/>
+    </row>
+    <row r="706" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A706"/>
+      <c r="F706" s="55"/>
+    </row>
+    <row r="707" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A707"/>
+      <c r="F707" s="55"/>
+    </row>
+    <row r="708" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A708"/>
+      <c r="F708" s="55"/>
+    </row>
+    <row r="709" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A709"/>
+      <c r="F709" s="55"/>
+    </row>
+    <row r="710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A710"/>
+      <c r="F710" s="55"/>
+    </row>
+    <row r="711" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A711"/>
+      <c r="F711" s="55"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{59E6726C-0839-4162-9FF1-1657CF96AFCB}">
+      <formula1>"?, kcal*Å^12/mol, kJ*nm^12/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{842B5519-800E-4032-B267-7C8A108080C5}">
+      <formula1>"Lennard-Jones (12-6) [A-B Form]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{34C173AC-5620-4E6B-AE8F-7EA648D43246}">
+      <formula1>$B$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{5BE516BC-2ADA-4ADE-BB35-BF8FF18122A7}">
+      <formula1>"?, kcal*Å^6/mol, kJ*nm^6/mol"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7F4F1D-08EB-4B7B-8B48-3727745CD76C}">
+  <sheetPr>
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1306,10 +5381,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -1862,20 +5937,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
     </row>
     <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -1891,64 +5966,64 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="41" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="39"/>
+    <row r="4" spans="1:4" s="37" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,17 +6121,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2333,17 +6408,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2620,20 +6695,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -2928,4 +7003,280 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B18951-00C9-4DCE-9582-2C01056EDACF}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{0CB10C05-A0A3-4F2A-9AEC-F40FA1C47675}">
+      <formula1>"?, ATDL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBEC09B-8297-4D8D-A8E3-380E64E4C5B9}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{DEC69AA4-2EF5-4F74-B509-9058309B55A5}">
+      <formula1>"?, Generic"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>